<commit_message>
updated results and minor bug
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2592"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2592" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="81">
   <si>
     <t>equals_Wrapper("")</t>
   </si>
@@ -224,13 +225,49 @@
     <t>containsKey_Wrapper</t>
   </si>
   <si>
-    <t>HTTP</t>
-  </si>
-  <si>
     <t>how scales with larger input size</t>
   </si>
   <si>
     <t>screencap of plugin</t>
+  </si>
+  <si>
+    <t>API/Sensor</t>
+  </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>HashMap/Dictionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerometer </t>
+  </si>
+  <si>
+    <t>BTLE</t>
+  </si>
+  <si>
+    <t>Wifi</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Overall Yes Rank 1 Only</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Overall Yes Rank 1 and 2</t>
+  </si>
+  <si>
+    <t>Rank 1 + 2 Yes</t>
+  </si>
+  <si>
+    <t>Rank 1</t>
+  </si>
+  <si>
+    <t>Rank 2</t>
   </si>
 </sst>
 </file>
@@ -548,21 +585,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:L66"/>
+  <dimension ref="C3:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="8" max="8" width="7.77734375" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>25</v>
       </c>
@@ -570,24 +608,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
       <c r="L4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>34</v>
       </c>
@@ -600,14 +632,11 @@
       <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
       <c r="L5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>31</v>
       </c>
@@ -617,11 +646,8 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="H6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>2</v>
       </c>
@@ -632,7 +658,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>3</v>
       </c>
@@ -643,7 +669,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>4</v>
       </c>
@@ -654,7 +680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>5</v>
       </c>
@@ -665,7 +691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>6</v>
       </c>
@@ -675,8 +701,17 @@
       <c r="F11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>7</v>
       </c>
@@ -686,8 +721,38 @@
       <c r="F12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>8</v>
       </c>
@@ -697,8 +762,41 @@
       <c r="F13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13">
+        <v>25</v>
+      </c>
+      <c r="I13">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>8</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>9</v>
       </c>
@@ -708,8 +806,41 @@
       <c r="F14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
+      <c r="Q14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>10</v>
       </c>
@@ -719,8 +850,41 @@
       <c r="F15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>3</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>11</v>
       </c>
@@ -730,8 +894,41 @@
       <c r="F16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>12</v>
       </c>
@@ -741,8 +938,41 @@
       <c r="F17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>13</v>
       </c>
@@ -752,8 +982,41 @@
       <c r="F18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>14</v>
       </c>
@@ -763,8 +1026,41 @@
       <c r="F19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>4</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>15</v>
       </c>
@@ -774,8 +1070,45 @@
       <c r="F20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20">
+        <v>75</v>
+      </c>
+      <c r="I20">
+        <f>SUM(I13:I19)</f>
+        <v>56</v>
+      </c>
+      <c r="J20">
+        <v>14</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f>SUM(M13:M19)</f>
+        <v>32</v>
+      </c>
+      <c r="N20">
+        <f>14</f>
+        <v>14</v>
+      </c>
+      <c r="O20">
+        <v>15</v>
+      </c>
+      <c r="P20">
+        <v>16</v>
+      </c>
+      <c r="Q20">
+        <f>SUM(Q13:Q19)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>16</v>
       </c>
@@ -785,8 +1118,15 @@
       <c r="F21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21">
+        <f>56/75</f>
+        <v>0.7466666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>17</v>
       </c>
@@ -796,8 +1136,15 @@
       <c r="F22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22">
+        <f>65/75</f>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>18</v>
       </c>
@@ -808,7 +1155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>19</v>
       </c>
@@ -819,7 +1166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>20</v>
       </c>
@@ -830,7 +1177,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>21</v>
       </c>
@@ -841,7 +1188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>22</v>
       </c>
@@ -852,7 +1199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>23</v>
       </c>
@@ -863,7 +1210,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>24</v>
       </c>
@@ -874,7 +1221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>35</v>
       </c>
@@ -888,7 +1235,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>36</v>
       </c>
@@ -1269,4 +1616,364 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C3:C9)</f>
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f>SUM(G3:G9)</f>
+        <v>32</v>
+      </c>
+      <c r="H10">
+        <f>14</f>
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <v>16</v>
+      </c>
+      <c r="K10">
+        <f>SUM(K3:K9)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <f>56/75</f>
+        <v>0.7466666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12">
+        <f>65/75</f>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>